<commit_message>
scaling mostly implemented, but still needs some powers sorted out
</commit_message>
<xml_diff>
--- a/PartBalance.xlsx
+++ b/PartBalance.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -10,12 +10,12 @@
     <sheet name="BaseStats" sheetId="1" r:id="rId1"/>
     <sheet name="ScaledStats" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="46">
   <si>
     <t>Repulsor</t>
   </si>
@@ -107,9 +107,6 @@
     <t>mTorque</t>
   </si>
   <si>
-    <t>mPwr</t>
-  </si>
-  <si>
     <t>mRPM</t>
   </si>
   <si>
@@ -150,6 +147,12 @@
   </si>
   <si>
     <t>max rpm</t>
+  </si>
+  <si>
+    <t>EC/s</t>
+  </si>
+  <si>
+    <t>mEff</t>
   </si>
 </sst>
 </file>
@@ -193,7 +196,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -563,21 +566,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -666,23 +697,61 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -745,7 +814,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -780,7 +849,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -989,10 +1058,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V19"/>
+  <dimension ref="A1:W19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R23" sqref="R23"/>
+      <selection activeCell="S23" sqref="S23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1013,1224 +1082,1279 @@
     <col min="14" max="14" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="70.42578125" customWidth="1"/>
+    <col min="17" max="18" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="70.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="1" t="s">
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="1" t="s">
+      <c r="N1" s="52"/>
+      <c r="O1" s="52"/>
+      <c r="P1" s="52"/>
+      <c r="Q1" s="52"/>
+      <c r="R1" s="52"/>
+      <c r="S1" s="53"/>
+      <c r="T1" s="42" t="s">
+        <v>32</v>
+      </c>
+      <c r="U1" s="44"/>
+      <c r="V1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="T1" s="3"/>
-      <c r="U1" s="6" t="s">
+      <c r="W1" s="45" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="33" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="K2" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="L2" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" s="54" t="s">
+        <v>45</v>
+      </c>
+      <c r="O2" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="P2" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q2" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="R2" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="S2" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="T2" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="U2" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="V2" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="V1" s="40" t="s">
-        <v>39</v>
-      </c>
+      <c r="W2" s="46"/>
     </row>
-    <row r="2" spans="1:22" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="35" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="36" t="s">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="E3" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="F3" s="6">
+        <v>3.5</v>
+      </c>
+      <c r="G3" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="H3" s="6">
+        <v>2</v>
+      </c>
+      <c r="I3" s="6">
+        <v>10</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="M3" s="8">
+        <v>0</v>
+      </c>
+      <c r="N3" s="55">
+        <v>1</v>
+      </c>
+      <c r="O3" s="6">
+        <v>0</v>
+      </c>
+      <c r="P3" s="6">
         <v>4</v>
       </c>
-      <c r="D2" s="36" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="36" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="36" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="36" t="s">
-        <v>43</v>
-      </c>
-      <c r="K2" s="42" t="s">
-        <v>44</v>
-      </c>
-      <c r="L2" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="N2" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="O2" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="P2" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q2" s="38" t="s">
-        <v>40</v>
-      </c>
-      <c r="R2" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="S2" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="T2" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="U2" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="V2" s="41"/>
+      <c r="Q3" s="9">
+        <f>IFERROR(O3/P3/60*D3*2*PI(), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="R3" s="48">
+        <f>IFERROR(M3*P3/D3, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="S3" s="10">
+        <f>0.5*M3*0.5*O3/9.5488/N3</f>
+        <v>0</v>
+      </c>
+      <c r="T3" s="8">
+        <v>0</v>
+      </c>
+      <c r="U3" s="10">
+        <f t="shared" ref="U3:U5" si="0">T3*D3</f>
+        <v>0</v>
+      </c>
+      <c r="V3" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="W3" s="36"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="9">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="12"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="14">
         <v>0.2</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E4" s="14">
         <v>0.1</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F4" s="14">
         <v>3.5</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G4" s="14">
         <v>0.5</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H4" s="14">
         <v>2</v>
       </c>
-      <c r="I3" s="9">
+      <c r="I4" s="14">
         <v>10</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J4" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="K3" s="43" t="s">
+      <c r="K4" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="L4" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="M3" s="11">
-        <v>0</v>
-      </c>
-      <c r="N3" s="12">
-        <f t="shared" ref="N3:N5" si="0">M3*1</f>
-        <v>0</v>
-      </c>
-      <c r="O3" s="9">
-        <v>0</v>
-      </c>
-      <c r="P3" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="12">
-        <f>IFERROR(O3/P3/60*D3*2*PI(), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="R3" s="13">
-        <f>IFERROR(M3*P3*D3, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="S3" s="11">
-        <v>0</v>
-      </c>
-      <c r="T3" s="13">
-        <f t="shared" ref="T3:T5" si="1">S3*D3</f>
-        <v>0</v>
-      </c>
-      <c r="U3" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="V3" s="39"/>
+      <c r="M4" s="16">
+        <v>0</v>
+      </c>
+      <c r="N4" s="56">
+        <v>1</v>
+      </c>
+      <c r="O4" s="14">
+        <v>0</v>
+      </c>
+      <c r="P4" s="14">
+        <v>4</v>
+      </c>
+      <c r="Q4" s="17">
+        <f t="shared" ref="Q4:Q19" si="1">IFERROR(O4/P4/60*D4*2*PI(), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="R4" s="49">
+        <f t="shared" ref="R4:R19" si="2">IFERROR(M4*P4/D4, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="S4" s="18">
+        <f t="shared" ref="S4:S19" si="3">0.5*M4*0.5*O4/9.5488/N4</f>
+        <v>0</v>
+      </c>
+      <c r="T4" s="16">
+        <v>0</v>
+      </c>
+      <c r="U4" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V4" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="W4" s="1"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="17">
-        <v>0.2</v>
-      </c>
-      <c r="E4" s="17">
-        <v>0.1</v>
-      </c>
-      <c r="F4" s="17">
-        <v>3.5</v>
-      </c>
-      <c r="G4" s="17">
-        <v>0.5</v>
-      </c>
-      <c r="H4" s="17">
-        <v>2</v>
-      </c>
-      <c r="I4" s="17">
-        <v>10</v>
-      </c>
-      <c r="J4" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="K4" s="44" t="s">
-        <v>28</v>
-      </c>
-      <c r="L4" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="M4" s="19">
-        <v>0</v>
-      </c>
-      <c r="N4" s="20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O4" s="17">
-        <v>0</v>
-      </c>
-      <c r="P4" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="20">
-        <f t="shared" ref="Q4:Q19" si="2">IFERROR(O4/P4/60*D4*2*PI(), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="R4" s="21">
-        <f t="shared" ref="R4:R19" si="3">IFERROR(M4*P4*D4, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="S4" s="19">
-        <v>0</v>
-      </c>
-      <c r="T4" s="21">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="U4" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="V4" s="4"/>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="17">
+      <c r="B5" s="12"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="14">
         <v>0.2</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="14">
         <v>0.1</v>
       </c>
-      <c r="F5" s="17">
+      <c r="F5" s="14">
         <v>0.75</v>
       </c>
-      <c r="G5" s="17">
+      <c r="G5" s="14">
         <v>0.5</v>
       </c>
-      <c r="H5" s="17">
+      <c r="H5" s="14">
         <v>2</v>
       </c>
-      <c r="I5" s="17">
+      <c r="I5" s="14">
         <v>10</v>
       </c>
-      <c r="J5" s="17" t="s">
+      <c r="J5" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="44" t="s">
+      <c r="K5" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="L5" s="18" t="s">
+      <c r="L5" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="M5" s="19">
-        <v>0</v>
-      </c>
-      <c r="N5" s="20">
+      <c r="M5" s="16">
+        <v>0</v>
+      </c>
+      <c r="N5" s="56">
+        <v>1</v>
+      </c>
+      <c r="O5" s="14">
+        <v>0</v>
+      </c>
+      <c r="P5" s="14">
+        <v>4</v>
+      </c>
+      <c r="Q5" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R5" s="49">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S5" s="18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T5" s="16">
+        <v>0</v>
+      </c>
+      <c r="U5" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O5" s="17">
-        <v>0</v>
-      </c>
-      <c r="P5" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="20">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R5" s="21">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="S5" s="19">
-        <v>0</v>
-      </c>
-      <c r="T5" s="21">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="U5" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="V5" s="4"/>
+      <c r="V5" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="W5" s="1"/>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="17">
+      <c r="B6" s="12"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="14">
         <v>0.375</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E6" s="14">
         <v>0.04</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6" s="14">
         <v>0.15</v>
       </c>
-      <c r="G6" s="17">
+      <c r="G6" s="14">
         <v>0.1</v>
       </c>
-      <c r="H6" s="17">
+      <c r="H6" s="14">
         <v>0.1</v>
       </c>
-      <c r="I6" s="17">
+      <c r="I6" s="14">
         <v>10</v>
       </c>
-      <c r="J6" s="16">
+      <c r="J6" s="13">
         <f>K6*D6*2*PI()/60</f>
         <v>23.561944901923447</v>
       </c>
-      <c r="K6" s="45">
+      <c r="K6" s="40">
         <v>600</v>
       </c>
-      <c r="L6" s="23"/>
-      <c r="M6" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="N6" s="20">
-        <f>M6*1</f>
-        <v>0.1</v>
-      </c>
-      <c r="O6" s="17">
-        <v>1000</v>
-      </c>
-      <c r="P6" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="20">
+      <c r="L6" s="20"/>
+      <c r="M6" s="16">
+        <v>1</v>
+      </c>
+      <c r="N6" s="56">
+        <v>1</v>
+      </c>
+      <c r="O6" s="14">
+        <v>2500</v>
+      </c>
+      <c r="P6" s="14">
+        <v>4</v>
+      </c>
+      <c r="Q6" s="17">
+        <f t="shared" si="1"/>
+        <v>24.543692606170257</v>
+      </c>
+      <c r="R6" s="49">
         <f t="shared" si="2"/>
-        <v>39.269908169872416</v>
-      </c>
-      <c r="R6" s="21">
+        <v>10.666666666666666</v>
+      </c>
+      <c r="S6" s="18">
         <f t="shared" si="3"/>
-        <v>3.7500000000000006E-2</v>
-      </c>
-      <c r="S6" s="19">
-        <v>0</v>
-      </c>
-      <c r="T6" s="21">
-        <f>S6*D6</f>
-        <v>0</v>
-      </c>
-      <c r="U6" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="V6" s="4"/>
+        <v>65.453250670241289</v>
+      </c>
+      <c r="T6" s="16">
+        <v>0</v>
+      </c>
+      <c r="U6" s="18">
+        <f>T6*D6</f>
+        <v>0</v>
+      </c>
+      <c r="V6" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="W6" s="1"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="17">
+      <c r="B7" s="12"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="14">
         <v>0.09</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="14">
         <v>0.04</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="14">
         <v>0.15</v>
       </c>
-      <c r="G7" s="17">
+      <c r="G7" s="14">
         <v>0.1</v>
       </c>
-      <c r="H7" s="17">
+      <c r="H7" s="14">
         <v>0.1</v>
       </c>
-      <c r="I7" s="17">
+      <c r="I7" s="14">
         <v>2.5</v>
       </c>
-      <c r="J7" s="16">
+      <c r="J7" s="13">
         <f t="shared" ref="J7:J19" si="4">K7*D7*2*PI()/60</f>
         <v>5.6548667764616276</v>
       </c>
-      <c r="K7" s="45">
+      <c r="K7" s="40">
         <v>600</v>
       </c>
-      <c r="L7" s="23"/>
-      <c r="M7" s="19">
-        <v>0</v>
-      </c>
-      <c r="N7" s="20">
-        <f t="shared" ref="N7:N19" si="5">M7*1</f>
-        <v>0</v>
-      </c>
-      <c r="O7" s="17">
-        <v>0</v>
-      </c>
-      <c r="P7" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="20">
+      <c r="L7" s="20"/>
+      <c r="M7" s="16">
+        <v>1</v>
+      </c>
+      <c r="N7" s="56">
+        <v>1</v>
+      </c>
+      <c r="O7" s="14">
+        <v>0</v>
+      </c>
+      <c r="P7" s="14">
+        <v>4</v>
+      </c>
+      <c r="Q7" s="17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="R7" s="49">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R7" s="21">
+        <v>44.444444444444443</v>
+      </c>
+      <c r="S7" s="18">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="S7" s="19">
-        <v>0</v>
-      </c>
-      <c r="T7" s="21">
-        <f t="shared" ref="T7:T19" si="6">S7*D7</f>
-        <v>0</v>
-      </c>
-      <c r="U7" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="V7" s="4"/>
+      <c r="T7" s="16">
+        <v>0</v>
+      </c>
+      <c r="U7" s="18">
+        <f t="shared" ref="U7:U19" si="5">T7*D7</f>
+        <v>0</v>
+      </c>
+      <c r="V7" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="W7" s="1"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="17">
+      <c r="B8" s="12"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="14">
         <v>0.25</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="14">
         <v>0.04</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F8" s="14">
         <v>0.05</v>
       </c>
-      <c r="G8" s="17">
+      <c r="G8" s="14">
         <v>0.1</v>
       </c>
-      <c r="H8" s="17">
+      <c r="H8" s="14">
         <v>0.1</v>
       </c>
-      <c r="I8" s="17">
+      <c r="I8" s="14">
         <v>5</v>
       </c>
-      <c r="J8" s="16">
+      <c r="J8" s="13">
         <f t="shared" si="4"/>
         <v>15.707963267948966</v>
       </c>
-      <c r="K8" s="45">
+      <c r="K8" s="40">
         <v>600</v>
       </c>
-      <c r="L8" s="23"/>
-      <c r="M8" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="N8" s="20">
+      <c r="L8" s="20"/>
+      <c r="M8" s="16">
+        <v>1</v>
+      </c>
+      <c r="N8" s="56">
+        <v>1</v>
+      </c>
+      <c r="O8" s="14">
+        <v>2500</v>
+      </c>
+      <c r="P8" s="14">
+        <v>4</v>
+      </c>
+      <c r="Q8" s="17">
+        <f t="shared" si="1"/>
+        <v>16.362461737446839</v>
+      </c>
+      <c r="R8" s="49">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="S8" s="18">
+        <f t="shared" si="3"/>
+        <v>65.453250670241289</v>
+      </c>
+      <c r="T8" s="16">
+        <v>70</v>
+      </c>
+      <c r="U8" s="18">
         <f t="shared" si="5"/>
-        <v>0.1</v>
-      </c>
-      <c r="O8" s="17">
-        <v>1200</v>
-      </c>
-      <c r="P8" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q8" s="20">
-        <f t="shared" si="2"/>
-        <v>31.415926535897931</v>
-      </c>
-      <c r="R8" s="21">
-        <f t="shared" si="3"/>
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="S8" s="19">
-        <v>70</v>
-      </c>
-      <c r="T8" s="21">
-        <f t="shared" si="6"/>
         <v>17.5</v>
       </c>
-      <c r="U8" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="V8" s="4"/>
+      <c r="V8" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="W8" s="1"/>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="17">
+      <c r="B9" s="12"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="14">
         <v>0.25</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="14">
         <v>0.04</v>
       </c>
-      <c r="F9" s="17">
+      <c r="F9" s="14">
         <v>0.17499999999999999</v>
       </c>
-      <c r="G9" s="17">
+      <c r="G9" s="14">
         <v>0.1</v>
       </c>
-      <c r="H9" s="17">
+      <c r="H9" s="14">
         <v>0.1</v>
       </c>
-      <c r="I9" s="17">
+      <c r="I9" s="14">
         <v>2.5</v>
       </c>
-      <c r="J9" s="16">
+      <c r="J9" s="13">
         <f t="shared" si="4"/>
         <v>15.707963267948966</v>
       </c>
-      <c r="K9" s="45">
+      <c r="K9" s="40">
         <v>600</v>
       </c>
-      <c r="L9" s="23"/>
-      <c r="M9" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="N9" s="20">
+      <c r="L9" s="20"/>
+      <c r="M9" s="16">
+        <v>1</v>
+      </c>
+      <c r="N9" s="56">
+        <v>1</v>
+      </c>
+      <c r="O9" s="14">
+        <v>2500</v>
+      </c>
+      <c r="P9" s="14">
+        <v>4</v>
+      </c>
+      <c r="Q9" s="17">
+        <f t="shared" si="1"/>
+        <v>16.362461737446839</v>
+      </c>
+      <c r="R9" s="49">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="S9" s="18">
+        <f t="shared" si="3"/>
+        <v>65.453250670241289</v>
+      </c>
+      <c r="T9" s="16">
+        <v>70</v>
+      </c>
+      <c r="U9" s="18">
         <f t="shared" si="5"/>
-        <v>0.1</v>
-      </c>
-      <c r="O9" s="17">
-        <v>600</v>
-      </c>
-      <c r="P9" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q9" s="20">
-        <f t="shared" si="2"/>
-        <v>15.707963267948966</v>
-      </c>
-      <c r="R9" s="21">
-        <f t="shared" si="3"/>
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="S9" s="19">
-        <v>70</v>
-      </c>
-      <c r="T9" s="21">
-        <f t="shared" si="6"/>
         <v>17.5</v>
       </c>
-      <c r="U9" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="V9" s="4"/>
+      <c r="V9" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="W9" s="1"/>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="17">
+      <c r="B10" s="12"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="14">
         <v>0.3</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="14">
         <v>0.04</v>
       </c>
-      <c r="F10" s="17">
+      <c r="F10" s="14">
         <v>0.125</v>
       </c>
-      <c r="G10" s="17">
+      <c r="G10" s="14">
         <v>0.1</v>
       </c>
-      <c r="H10" s="17">
-        <v>1</v>
-      </c>
-      <c r="I10" s="17">
+      <c r="H10" s="14">
+        <v>1</v>
+      </c>
+      <c r="I10" s="14">
         <v>5</v>
       </c>
-      <c r="J10" s="16">
+      <c r="J10" s="13">
         <f t="shared" si="4"/>
         <v>18.849555921538759</v>
       </c>
-      <c r="K10" s="45">
+      <c r="K10" s="40">
         <v>600</v>
       </c>
-      <c r="L10" s="23"/>
-      <c r="M10" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="N10" s="20">
+      <c r="L10" s="20"/>
+      <c r="M10" s="16">
+        <v>1</v>
+      </c>
+      <c r="N10" s="56">
+        <v>1</v>
+      </c>
+      <c r="O10" s="14">
+        <v>2500</v>
+      </c>
+      <c r="P10" s="14">
+        <v>4</v>
+      </c>
+      <c r="Q10" s="17">
+        <f t="shared" si="1"/>
+        <v>19.634954084936204</v>
+      </c>
+      <c r="R10" s="49">
+        <f t="shared" si="2"/>
+        <v>13.333333333333334</v>
+      </c>
+      <c r="S10" s="18">
+        <f t="shared" si="3"/>
+        <v>65.453250670241289</v>
+      </c>
+      <c r="T10" s="16">
+        <v>12</v>
+      </c>
+      <c r="U10" s="18">
         <f t="shared" si="5"/>
-        <v>0.1</v>
-      </c>
-      <c r="O10" s="17">
-        <v>600</v>
-      </c>
-      <c r="P10" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q10" s="20">
-        <f t="shared" si="2"/>
-        <v>18.849555921538759</v>
-      </c>
-      <c r="R10" s="21">
-        <f t="shared" si="3"/>
-        <v>0.03</v>
-      </c>
-      <c r="S10" s="19">
-        <v>12</v>
-      </c>
-      <c r="T10" s="21">
-        <f t="shared" si="6"/>
         <v>3.5999999999999996</v>
       </c>
-      <c r="U10" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="V10" s="4"/>
+      <c r="V10" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="W10" s="1"/>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="17">
+      <c r="B11" s="12"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="14">
         <v>1.3</v>
       </c>
-      <c r="E11" s="17">
+      <c r="E11" s="14">
         <v>0.2</v>
       </c>
-      <c r="F11" s="17">
+      <c r="F11" s="14">
         <v>0.35</v>
       </c>
-      <c r="G11" s="17">
-        <v>1</v>
-      </c>
-      <c r="H11" s="17">
+      <c r="G11" s="14">
+        <v>1</v>
+      </c>
+      <c r="H11" s="14">
         <v>3</v>
       </c>
-      <c r="I11" s="17">
+      <c r="I11" s="14">
         <v>20</v>
       </c>
-      <c r="J11" s="16">
+      <c r="J11" s="13">
         <f t="shared" si="4"/>
         <v>81.681408993334614</v>
       </c>
-      <c r="K11" s="45">
+      <c r="K11" s="40">
         <v>600</v>
       </c>
-      <c r="L11" s="23"/>
-      <c r="M11" s="19">
+      <c r="L11" s="20"/>
+      <c r="M11" s="16">
         <v>30</v>
       </c>
-      <c r="N11" s="20">
+      <c r="N11" s="56">
+        <v>1</v>
+      </c>
+      <c r="O11" s="14">
+        <v>200</v>
+      </c>
+      <c r="P11" s="14">
+        <v>4</v>
+      </c>
+      <c r="Q11" s="17">
+        <f t="shared" si="1"/>
+        <v>6.8067840827778863</v>
+      </c>
+      <c r="R11" s="49">
+        <f t="shared" si="2"/>
+        <v>92.307692307692307</v>
+      </c>
+      <c r="S11" s="18">
+        <f t="shared" si="3"/>
+        <v>157.0878016085791</v>
+      </c>
+      <c r="T11" s="16">
+        <v>100</v>
+      </c>
+      <c r="U11" s="18">
         <f t="shared" si="5"/>
-        <v>30</v>
-      </c>
-      <c r="O11" s="17">
-        <v>200</v>
-      </c>
-      <c r="P11" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q11" s="20">
-        <f t="shared" si="2"/>
-        <v>27.227136331111545</v>
-      </c>
-      <c r="R11" s="21">
-        <f t="shared" si="3"/>
-        <v>39</v>
-      </c>
-      <c r="S11" s="19">
-        <v>100</v>
-      </c>
-      <c r="T11" s="21">
-        <f t="shared" si="6"/>
         <v>130</v>
       </c>
-      <c r="U11" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="V11" s="4"/>
+      <c r="V11" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="W11" s="1"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="17">
+      <c r="B12" s="12"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="14">
         <v>0.13</v>
       </c>
-      <c r="E12" s="17">
+      <c r="E12" s="14">
         <v>0.04</v>
       </c>
-      <c r="F12" s="17">
+      <c r="F12" s="14">
         <v>0.05</v>
       </c>
-      <c r="G12" s="17">
+      <c r="G12" s="14">
         <v>0.1</v>
       </c>
-      <c r="H12" s="17">
+      <c r="H12" s="14">
         <v>0.1</v>
       </c>
-      <c r="I12" s="17">
+      <c r="I12" s="14">
         <v>2.5</v>
       </c>
-      <c r="J12" s="16">
+      <c r="J12" s="13">
         <f t="shared" si="4"/>
         <v>8.1681408993334621</v>
       </c>
-      <c r="K12" s="45">
+      <c r="K12" s="40">
         <v>600</v>
       </c>
-      <c r="L12" s="23"/>
-      <c r="M12" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="N12" s="20">
+      <c r="L12" s="20"/>
+      <c r="M12" s="16">
+        <v>1</v>
+      </c>
+      <c r="N12" s="56">
+        <v>1</v>
+      </c>
+      <c r="O12" s="14">
+        <v>2500</v>
+      </c>
+      <c r="P12" s="14">
+        <v>4</v>
+      </c>
+      <c r="Q12" s="17">
+        <f t="shared" si="1"/>
+        <v>8.5084801034723565</v>
+      </c>
+      <c r="R12" s="49">
+        <f t="shared" si="2"/>
+        <v>30.769230769230766</v>
+      </c>
+      <c r="S12" s="18">
+        <f t="shared" si="3"/>
+        <v>65.453250670241289</v>
+      </c>
+      <c r="T12" s="16">
+        <v>50</v>
+      </c>
+      <c r="U12" s="18">
         <f t="shared" si="5"/>
-        <v>0.1</v>
-      </c>
-      <c r="O12" s="17">
-        <v>800</v>
-      </c>
-      <c r="P12" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="20">
-        <f t="shared" si="2"/>
-        <v>10.890854532444617</v>
-      </c>
-      <c r="R12" s="21">
-        <f t="shared" si="3"/>
-        <v>1.3000000000000001E-2</v>
-      </c>
-      <c r="S12" s="19">
-        <v>50</v>
-      </c>
-      <c r="T12" s="21">
-        <f t="shared" si="6"/>
         <v>6.5</v>
       </c>
-      <c r="U12" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="V12" s="4"/>
+      <c r="V12" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="W12" s="1"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="17">
+      <c r="B13" s="12"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="14">
         <v>0.14000000000000001</v>
       </c>
-      <c r="E13" s="17">
+      <c r="E13" s="14">
         <v>0.04</v>
       </c>
-      <c r="F13" s="17">
+      <c r="F13" s="14">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="G13" s="17">
+      <c r="G13" s="14">
         <v>0.1</v>
       </c>
-      <c r="H13" s="17">
+      <c r="H13" s="14">
         <v>0.1</v>
       </c>
-      <c r="I13" s="17">
+      <c r="I13" s="14">
         <v>5</v>
       </c>
-      <c r="J13" s="16">
+      <c r="J13" s="13">
         <f t="shared" si="4"/>
         <v>8.7964594300514225</v>
       </c>
-      <c r="K13" s="45">
+      <c r="K13" s="40">
         <v>600</v>
       </c>
-      <c r="L13" s="23"/>
-      <c r="M13" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="N13" s="20">
+      <c r="L13" s="20"/>
+      <c r="M13" s="16">
+        <v>1</v>
+      </c>
+      <c r="N13" s="56">
+        <v>1</v>
+      </c>
+      <c r="O13" s="14">
+        <v>2500</v>
+      </c>
+      <c r="P13" s="14">
+        <v>4</v>
+      </c>
+      <c r="Q13" s="17">
+        <f t="shared" si="1"/>
+        <v>9.1629785729702302</v>
+      </c>
+      <c r="R13" s="49">
+        <f t="shared" si="2"/>
+        <v>28.571428571428569</v>
+      </c>
+      <c r="S13" s="18">
+        <f t="shared" si="3"/>
+        <v>65.453250670241289</v>
+      </c>
+      <c r="T13" s="16">
+        <v>50</v>
+      </c>
+      <c r="U13" s="18">
         <f t="shared" si="5"/>
-        <v>0.1</v>
-      </c>
-      <c r="O13" s="17">
-        <v>1000</v>
-      </c>
-      <c r="P13" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q13" s="20">
-        <f t="shared" si="2"/>
-        <v>14.660765716752371</v>
-      </c>
-      <c r="R13" s="21">
-        <f t="shared" si="3"/>
-        <v>1.4000000000000002E-2</v>
-      </c>
-      <c r="S13" s="19">
-        <v>50</v>
-      </c>
-      <c r="T13" s="21">
-        <f t="shared" si="6"/>
         <v>7.0000000000000009</v>
       </c>
-      <c r="U13" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="V13" s="4"/>
+      <c r="V13" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="W13" s="1"/>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="17">
+      <c r="B14" s="12"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="14">
         <v>0.16</v>
       </c>
-      <c r="E14" s="17">
+      <c r="E14" s="14">
         <v>0.04</v>
       </c>
-      <c r="F14" s="17">
+      <c r="F14" s="14">
         <v>0.1</v>
       </c>
-      <c r="G14" s="17">
+      <c r="G14" s="14">
         <v>0.1</v>
       </c>
-      <c r="H14" s="17">
+      <c r="H14" s="14">
         <v>0.1</v>
       </c>
-      <c r="I14" s="17">
+      <c r="I14" s="14">
         <v>5</v>
       </c>
-      <c r="J14" s="16">
+      <c r="J14" s="13">
         <f t="shared" si="4"/>
         <v>10.053096491487338</v>
       </c>
-      <c r="K14" s="45">
+      <c r="K14" s="40">
         <v>600</v>
       </c>
-      <c r="L14" s="23"/>
-      <c r="M14" s="19">
-        <v>1</v>
-      </c>
-      <c r="N14" s="20">
+      <c r="L14" s="20"/>
+      <c r="M14" s="16">
+        <v>1</v>
+      </c>
+      <c r="N14" s="56">
+        <v>1</v>
+      </c>
+      <c r="O14" s="14">
+        <v>2500</v>
+      </c>
+      <c r="P14" s="14">
+        <v>4</v>
+      </c>
+      <c r="Q14" s="17">
+        <f t="shared" si="1"/>
+        <v>10.471975511965976</v>
+      </c>
+      <c r="R14" s="49">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="S14" s="18">
+        <f t="shared" si="3"/>
+        <v>65.453250670241289</v>
+      </c>
+      <c r="T14" s="16">
+        <v>12</v>
+      </c>
+      <c r="U14" s="18">
         <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="O14" s="17">
-        <v>600</v>
-      </c>
-      <c r="P14" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q14" s="20">
-        <f t="shared" si="2"/>
-        <v>10.053096491487338</v>
-      </c>
-      <c r="R14" s="21">
-        <f t="shared" si="3"/>
-        <v>0.16</v>
-      </c>
-      <c r="S14" s="19">
-        <v>12</v>
-      </c>
-      <c r="T14" s="21">
-        <f t="shared" si="6"/>
         <v>1.92</v>
       </c>
-      <c r="U14" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="V14" s="4"/>
+      <c r="V14" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="W14" s="1"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="17">
+      <c r="B15" s="12"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="14">
         <v>0.22</v>
       </c>
-      <c r="E15" s="17">
+      <c r="E15" s="14">
         <v>0.04</v>
       </c>
-      <c r="F15" s="17">
+      <c r="F15" s="14">
         <v>0.14000000000000001</v>
       </c>
-      <c r="G15" s="17">
+      <c r="G15" s="14">
         <v>0.1</v>
       </c>
-      <c r="H15" s="17">
+      <c r="H15" s="14">
         <v>0.1</v>
       </c>
-      <c r="I15" s="17">
+      <c r="I15" s="14">
         <v>2.5</v>
       </c>
-      <c r="J15" s="16">
+      <c r="J15" s="13">
         <f t="shared" si="4"/>
         <v>13.82300767579509</v>
       </c>
-      <c r="K15" s="45">
+      <c r="K15" s="40">
         <v>600</v>
       </c>
-      <c r="L15" s="23"/>
-      <c r="M15" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="N15" s="20">
+      <c r="L15" s="20"/>
+      <c r="M15" s="16">
+        <v>1</v>
+      </c>
+      <c r="N15" s="56">
+        <v>1</v>
+      </c>
+      <c r="O15" s="14">
+        <v>2500</v>
+      </c>
+      <c r="P15" s="14">
+        <v>4</v>
+      </c>
+      <c r="Q15" s="17">
+        <f t="shared" si="1"/>
+        <v>14.398966328953218</v>
+      </c>
+      <c r="R15" s="49">
+        <f t="shared" si="2"/>
+        <v>18.181818181818183</v>
+      </c>
+      <c r="S15" s="18">
+        <f t="shared" si="3"/>
+        <v>65.453250670241289</v>
+      </c>
+      <c r="T15" s="16">
+        <v>12</v>
+      </c>
+      <c r="U15" s="18">
         <f t="shared" si="5"/>
-        <v>0.1</v>
-      </c>
-      <c r="O15" s="17">
-        <v>600</v>
-      </c>
-      <c r="P15" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q15" s="20">
-        <f t="shared" si="2"/>
-        <v>13.823007675795091</v>
-      </c>
-      <c r="R15" s="21">
-        <f t="shared" si="3"/>
-        <v>2.2000000000000002E-2</v>
-      </c>
-      <c r="S15" s="19">
-        <v>12</v>
-      </c>
-      <c r="T15" s="21">
-        <f t="shared" si="6"/>
         <v>2.64</v>
       </c>
-      <c r="U15" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="V15" s="4"/>
+      <c r="V15" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="W15" s="1"/>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="17">
+      <c r="B16" s="12"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="14">
         <v>1.38</v>
       </c>
-      <c r="E16" s="17">
+      <c r="E16" s="14">
         <v>0.25</v>
       </c>
-      <c r="F16" s="17">
+      <c r="F16" s="14">
         <v>0.35</v>
       </c>
-      <c r="G16" s="17">
-        <v>1</v>
-      </c>
-      <c r="H16" s="17">
+      <c r="G16" s="14">
+        <v>1</v>
+      </c>
+      <c r="H16" s="14">
         <v>10</v>
       </c>
-      <c r="I16" s="17">
+      <c r="I16" s="14">
         <v>20</v>
       </c>
-      <c r="J16" s="16">
+      <c r="J16" s="13">
         <f t="shared" si="4"/>
         <v>86.707957239078283</v>
       </c>
-      <c r="K16" s="45">
+      <c r="K16" s="40">
         <v>600</v>
       </c>
-      <c r="L16" s="23"/>
-      <c r="M16" s="19">
-        <v>5</v>
-      </c>
-      <c r="N16" s="20">
+      <c r="L16" s="20"/>
+      <c r="M16" s="16">
+        <v>1</v>
+      </c>
+      <c r="N16" s="56">
+        <v>1</v>
+      </c>
+      <c r="O16" s="14">
+        <v>2500</v>
+      </c>
+      <c r="P16" s="14">
+        <v>4</v>
+      </c>
+      <c r="Q16" s="17">
+        <f t="shared" si="1"/>
+        <v>90.320788790706544</v>
+      </c>
+      <c r="R16" s="49">
+        <f t="shared" si="2"/>
+        <v>2.8985507246376816</v>
+      </c>
+      <c r="S16" s="18">
+        <f t="shared" si="3"/>
+        <v>65.453250670241289</v>
+      </c>
+      <c r="T16" s="16">
+        <v>100</v>
+      </c>
+      <c r="U16" s="18">
         <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="O16" s="17">
-        <v>2500</v>
-      </c>
-      <c r="P16" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q16" s="20">
-        <f t="shared" si="2"/>
-        <v>361.28315516282618</v>
-      </c>
-      <c r="R16" s="21">
-        <f t="shared" si="3"/>
-        <v>6.8999999999999995</v>
-      </c>
-      <c r="S16" s="19">
-        <v>100</v>
-      </c>
-      <c r="T16" s="21">
-        <f t="shared" si="6"/>
         <v>138</v>
       </c>
-      <c r="U16" s="22">
+      <c r="V16" s="19">
         <v>40</v>
       </c>
-      <c r="V16" s="4"/>
+      <c r="W16" s="1"/>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="15"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="17">
+      <c r="B17" s="12"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="14">
         <v>0.52</v>
       </c>
-      <c r="E17" s="17">
+      <c r="E17" s="14">
         <v>0.08</v>
       </c>
-      <c r="F17" s="17">
+      <c r="F17" s="14">
         <v>0.68</v>
       </c>
-      <c r="G17" s="17">
+      <c r="G17" s="14">
         <v>0.5</v>
       </c>
-      <c r="H17" s="17">
+      <c r="H17" s="14">
         <v>2</v>
       </c>
-      <c r="I17" s="17">
+      <c r="I17" s="14">
         <v>10</v>
       </c>
-      <c r="J17" s="16">
+      <c r="J17" s="13">
         <f t="shared" si="4"/>
         <v>32.672563597333848</v>
       </c>
-      <c r="K17" s="45">
+      <c r="K17" s="40">
         <v>600</v>
       </c>
-      <c r="L17" s="23"/>
-      <c r="M17" s="19">
-        <v>1</v>
-      </c>
-      <c r="N17" s="20">
+      <c r="L17" s="20"/>
+      <c r="M17" s="16">
+        <v>1</v>
+      </c>
+      <c r="N17" s="56">
+        <v>1</v>
+      </c>
+      <c r="O17" s="14">
+        <v>2500</v>
+      </c>
+      <c r="P17" s="14">
+        <v>4</v>
+      </c>
+      <c r="Q17" s="17">
+        <f t="shared" si="1"/>
+        <v>34.033920413889426</v>
+      </c>
+      <c r="R17" s="49">
+        <f t="shared" si="2"/>
+        <v>7.6923076923076916</v>
+      </c>
+      <c r="S17" s="18">
+        <f t="shared" si="3"/>
+        <v>65.453250670241289</v>
+      </c>
+      <c r="T17" s="16">
+        <v>80</v>
+      </c>
+      <c r="U17" s="18">
         <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="O17" s="17">
-        <v>425</v>
-      </c>
-      <c r="P17" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q17" s="20">
-        <f t="shared" si="2"/>
-        <v>23.143065881444809</v>
-      </c>
-      <c r="R17" s="21">
-        <f t="shared" si="3"/>
-        <v>0.52</v>
-      </c>
-      <c r="S17" s="19">
-        <v>80</v>
-      </c>
-      <c r="T17" s="21">
-        <f t="shared" si="6"/>
         <v>41.6</v>
       </c>
-      <c r="U17" s="22">
+      <c r="V17" s="19">
         <v>20</v>
       </c>
-      <c r="V17" s="4"/>
+      <c r="W17" s="1"/>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="15"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="17">
+      <c r="B18" s="12"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="14">
         <v>0.34399999999999997</v>
       </c>
-      <c r="E18" s="17">
+      <c r="E18" s="14">
         <v>0.04</v>
       </c>
-      <c r="F18" s="17">
+      <c r="F18" s="14">
         <v>0.21</v>
       </c>
-      <c r="G18" s="17">
+      <c r="G18" s="14">
         <v>0.1</v>
       </c>
-      <c r="H18" s="17">
-        <v>1</v>
-      </c>
-      <c r="I18" s="17">
+      <c r="H18" s="14">
+        <v>1</v>
+      </c>
+      <c r="I18" s="14">
         <v>5</v>
       </c>
-      <c r="J18" s="16">
+      <c r="J18" s="13">
         <f t="shared" si="4"/>
         <v>21.614157456697775</v>
       </c>
-      <c r="K18" s="45">
+      <c r="K18" s="40">
         <v>600</v>
       </c>
-      <c r="L18" s="23"/>
-      <c r="M18" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="N18" s="20">
+      <c r="L18" s="20"/>
+      <c r="M18" s="16">
+        <v>1</v>
+      </c>
+      <c r="N18" s="56">
+        <v>1</v>
+      </c>
+      <c r="O18" s="14">
+        <v>2500</v>
+      </c>
+      <c r="P18" s="14">
+        <v>4</v>
+      </c>
+      <c r="Q18" s="17">
+        <f t="shared" si="1"/>
+        <v>22.51474735072685</v>
+      </c>
+      <c r="R18" s="49">
+        <f t="shared" si="2"/>
+        <v>11.627906976744187</v>
+      </c>
+      <c r="S18" s="18">
+        <f t="shared" si="3"/>
+        <v>65.453250670241289</v>
+      </c>
+      <c r="T18" s="16">
+        <v>12</v>
+      </c>
+      <c r="U18" s="18">
         <f t="shared" si="5"/>
-        <v>0.5</v>
-      </c>
-      <c r="O18" s="17">
-        <v>600</v>
-      </c>
-      <c r="P18" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q18" s="20">
-        <f t="shared" si="2"/>
-        <v>21.614157456697775</v>
-      </c>
-      <c r="R18" s="21">
-        <f t="shared" si="3"/>
-        <v>0.17199999999999999</v>
-      </c>
-      <c r="S18" s="19">
-        <v>12</v>
-      </c>
-      <c r="T18" s="21">
-        <f t="shared" si="6"/>
         <v>4.1280000000000001</v>
       </c>
-      <c r="U18" s="22">
+      <c r="V18" s="19">
         <v>40</v>
       </c>
-      <c r="V18" s="4"/>
+      <c r="W18" s="1"/>
     </row>
-    <row r="19" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="24"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="26">
+      <c r="B19" s="21"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="23">
         <v>0.21</v>
       </c>
-      <c r="E19" s="26">
+      <c r="E19" s="23">
         <v>0.04</v>
       </c>
-      <c r="F19" s="26">
+      <c r="F19" s="23">
         <v>0.1</v>
       </c>
-      <c r="G19" s="26">
+      <c r="G19" s="23">
         <v>0.1</v>
       </c>
-      <c r="H19" s="26">
+      <c r="H19" s="23">
         <v>0.5</v>
       </c>
-      <c r="I19" s="26">
+      <c r="I19" s="23">
         <v>2</v>
       </c>
-      <c r="J19" s="25">
+      <c r="J19" s="22">
         <f t="shared" si="4"/>
         <v>13.194689145077131</v>
       </c>
-      <c r="K19" s="46">
+      <c r="K19" s="41">
         <v>600</v>
       </c>
-      <c r="L19" s="27"/>
-      <c r="M19" s="28">
-        <v>1</v>
-      </c>
-      <c r="N19" s="29">
+      <c r="L19" s="24"/>
+      <c r="M19" s="25">
+        <v>1</v>
+      </c>
+      <c r="N19" s="57">
+        <v>1</v>
+      </c>
+      <c r="O19" s="23">
+        <v>2500</v>
+      </c>
+      <c r="P19" s="23">
+        <v>4</v>
+      </c>
+      <c r="Q19" s="26">
+        <f t="shared" si="1"/>
+        <v>13.744467859455344</v>
+      </c>
+      <c r="R19" s="50">
+        <f t="shared" si="2"/>
+        <v>19.047619047619047</v>
+      </c>
+      <c r="S19" s="27">
+        <f t="shared" si="3"/>
+        <v>65.453250670241289</v>
+      </c>
+      <c r="T19" s="25">
+        <v>80</v>
+      </c>
+      <c r="U19" s="27">
         <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="O19" s="26">
-        <v>600</v>
-      </c>
-      <c r="P19" s="26">
-        <v>1</v>
-      </c>
-      <c r="Q19" s="29">
-        <f t="shared" si="2"/>
-        <v>13.194689145077131</v>
-      </c>
-      <c r="R19" s="30">
-        <f t="shared" si="3"/>
-        <v>0.21</v>
-      </c>
-      <c r="S19" s="28">
-        <v>80</v>
-      </c>
-      <c r="T19" s="30">
-        <f t="shared" si="6"/>
         <v>16.8</v>
       </c>
-      <c r="U19" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="V19" s="5"/>
+      <c r="V19" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="W19" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="M1:R1"/>
     <mergeCell ref="B1:L1"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="V1:V2"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="W1:W2"/>
+    <mergeCell ref="M1:S1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
initial bit of work on getting speed to matter as far as wear/load/breaking goes under 'simple' damage model
</commit_message>
<xml_diff>
--- a/PartBalance.xlsx
+++ b/PartBalance.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -10,12 +10,12 @@
     <sheet name="BaseStats" sheetId="1" r:id="rId1"/>
     <sheet name="ScaledStats" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="49">
   <si>
     <t>Repulsor</t>
   </si>
@@ -153,6 +153,15 @@
   </si>
   <si>
     <t>mEff</t>
+  </si>
+  <si>
+    <t>mPwr</t>
+  </si>
+  <si>
+    <t>m/s @ mLoad</t>
+  </si>
+  <si>
+    <t>t for 1g</t>
   </si>
 </sst>
 </file>
@@ -607,7 +616,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -627,9 +636,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -707,7 +713,18 @@
     <xf numFmtId="2" fontId="0" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -725,16 +742,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -744,14 +751,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -814,7 +817,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -849,7 +852,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1058,10 +1061,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W19"/>
+  <dimension ref="A1:Z19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S23" sqref="S23"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1081,29 +1084,32 @@
     <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.5703125" customWidth="1"/>
+    <col min="17" max="17" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="70.42578125" customWidth="1"/>
+    <col min="23" max="23" width="7" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="70.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="42" t="s">
+    <row r="1" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="44"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="48"/>
       <c r="M1" s="51" t="s">
         <v>26</v>
       </c>
@@ -1112,85 +1118,96 @@
       <c r="P1" s="52"/>
       <c r="Q1" s="52"/>
       <c r="R1" s="52"/>
-      <c r="S1" s="53"/>
-      <c r="T1" s="42" t="s">
+      <c r="S1" s="52"/>
+      <c r="T1" s="52"/>
+      <c r="U1" s="53"/>
+      <c r="V1" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="U1" s="44"/>
-      <c r="V1" s="3" t="s">
+      <c r="W1" s="48"/>
+      <c r="X1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="W1" s="45" t="s">
+      <c r="Y1" s="49" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="32" t="s">
+    <row r="2" spans="1:26" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="33" t="s">
+      <c r="D2" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="E2" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="33" t="s">
+      <c r="F2" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="33" t="s">
+      <c r="G2" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="33" t="s">
+      <c r="H2" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="33" t="s">
+      <c r="I2" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="33" t="s">
+      <c r="J2" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="K2" s="37" t="s">
+      <c r="K2" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="L2" s="34" t="s">
+      <c r="L2" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="32" t="s">
+      <c r="M2" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="N2" s="54" t="s">
+      <c r="N2" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="O2" s="33" t="s">
+      <c r="O2" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="P2" s="33" t="s">
+      <c r="P2" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q2" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="Q2" s="35" t="s">
+      <c r="R2" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="R2" s="47" t="s">
+      <c r="S2" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="S2" s="30" t="s">
+      <c r="T2" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="T2" s="29" t="s">
+      <c r="U2" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="V2" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="U2" s="30" t="s">
+      <c r="W2" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="V2" s="31" t="s">
+      <c r="X2" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="W2" s="46"/>
+      <c r="Y2" s="50"/>
+      <c r="Z2" t="s">
+        <v>48</v>
+      </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1217,1144 +1234,1259 @@
       <c r="J3" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="K3" s="38" t="s">
+      <c r="K3" s="37" t="s">
         <v>28</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="M3" s="8">
-        <v>0</v>
-      </c>
-      <c r="N3" s="55">
+      <c r="M3" s="4">
+        <v>0</v>
+      </c>
+      <c r="N3" s="5">
+        <v>0.15</v>
+      </c>
+      <c r="O3" s="5">
+        <v>0</v>
+      </c>
+      <c r="P3" s="5">
         <v>1</v>
       </c>
-      <c r="O3" s="6">
-        <v>0</v>
-      </c>
-      <c r="P3" s="6">
-        <v>4</v>
-      </c>
-      <c r="Q3" s="9">
-        <f>IFERROR(O3/P3/60*D3*2*PI(), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="R3" s="48">
-        <f>IFERROR(M3*P3/D3, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="S3" s="10">
-        <f>0.5*M3*0.5*O3/9.5488/N3</f>
-        <v>0</v>
-      </c>
-      <c r="T3" s="8">
-        <v>0</v>
-      </c>
-      <c r="U3" s="10">
-        <f t="shared" ref="U3:U5" si="0">T3*D3</f>
-        <v>0</v>
-      </c>
-      <c r="V3" s="11" t="s">
+      <c r="Q3" s="5">
+        <v>8</v>
+      </c>
+      <c r="R3" s="5">
+        <f>IFERROR(O3/Q3/60*D3*2*PI(), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="S3" s="54">
+        <f>IFERROR(M3*Q3/D3, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T3" s="54">
+        <v>6.666666666666667</v>
+      </c>
+      <c r="U3" s="55">
+        <f>IFERROR(S3/I3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V3" s="8">
+        <v>0</v>
+      </c>
+      <c r="W3" s="9">
+        <f>V3*D3</f>
+        <v>0</v>
+      </c>
+      <c r="X3" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="W3" s="36"/>
+      <c r="Y3" s="35"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="14">
+      <c r="B4" s="11"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="13">
         <v>0.2</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="13">
         <v>0.1</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="13">
         <v>3.5</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4" s="13">
         <v>0.5</v>
       </c>
-      <c r="H4" s="14">
+      <c r="H4" s="13">
         <v>2</v>
       </c>
-      <c r="I4" s="14">
+      <c r="I4" s="13">
         <v>10</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="J4" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="K4" s="39" t="s">
+      <c r="K4" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="L4" s="15" t="s">
+      <c r="L4" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="M4" s="16">
-        <v>0</v>
-      </c>
-      <c r="N4" s="56">
+      <c r="M4" s="11">
+        <v>0</v>
+      </c>
+      <c r="N4" s="12">
+        <v>0.15</v>
+      </c>
+      <c r="O4" s="12">
+        <v>0</v>
+      </c>
+      <c r="P4" s="12">
         <v>1</v>
       </c>
-      <c r="O4" s="14">
-        <v>0</v>
-      </c>
-      <c r="P4" s="14">
-        <v>4</v>
-      </c>
-      <c r="Q4" s="17">
-        <f t="shared" ref="Q4:Q19" si="1">IFERROR(O4/P4/60*D4*2*PI(), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="R4" s="49">
-        <f t="shared" ref="R4:R19" si="2">IFERROR(M4*P4/D4, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="S4" s="18">
-        <f t="shared" ref="S4:S19" si="3">0.5*M4*0.5*O4/9.5488/N4</f>
-        <v>0</v>
-      </c>
-      <c r="T4" s="16">
-        <v>0</v>
-      </c>
-      <c r="U4" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="V4" s="19" t="s">
+      <c r="Q4" s="12">
+        <v>8</v>
+      </c>
+      <c r="R4" s="12">
+        <f t="shared" ref="R4:R19" si="0">IFERROR(O4/Q4/60*D4*2*PI(), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="S4" s="39">
+        <f t="shared" ref="S4:S19" si="1">IFERROR(M4*Q4/D4, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="T4" s="39">
+        <v>6.666666666666667</v>
+      </c>
+      <c r="U4" s="19">
+        <f t="shared" ref="U4:U19" si="2">IFERROR(S4/I4,0)</f>
+        <v>0</v>
+      </c>
+      <c r="V4" s="15">
+        <v>0</v>
+      </c>
+      <c r="W4" s="17">
+        <f>V4*D4</f>
+        <v>0</v>
+      </c>
+      <c r="X4" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="W4" s="1"/>
+      <c r="Y4" s="1"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="14">
+      <c r="B5" s="11"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="13">
         <v>0.2</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="13">
         <v>0.1</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="13">
         <v>0.75</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="13">
         <v>0.5</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="13">
         <v>2</v>
       </c>
-      <c r="I5" s="14">
+      <c r="I5" s="13">
         <v>10</v>
       </c>
-      <c r="J5" s="14" t="s">
+      <c r="J5" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="39" t="s">
+      <c r="K5" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="L5" s="15" t="s">
+      <c r="L5" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="M5" s="16">
-        <v>0</v>
-      </c>
-      <c r="N5" s="56">
+      <c r="M5" s="11">
+        <v>0</v>
+      </c>
+      <c r="N5" s="12">
+        <v>0.15</v>
+      </c>
+      <c r="O5" s="12">
+        <v>0</v>
+      </c>
+      <c r="P5" s="12">
         <v>1</v>
       </c>
-      <c r="O5" s="14">
-        <v>0</v>
-      </c>
-      <c r="P5" s="14">
-        <v>4</v>
-      </c>
-      <c r="Q5" s="17">
+      <c r="Q5" s="12">
+        <v>8</v>
+      </c>
+      <c r="R5" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S5" s="39">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R5" s="49">
+      <c r="T5" s="39">
+        <v>6.666666666666667</v>
+      </c>
+      <c r="U5" s="19">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S5" s="18">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="T5" s="16">
-        <v>0</v>
-      </c>
-      <c r="U5" s="18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="V5" s="19" t="s">
+      <c r="V5" s="15">
+        <v>0</v>
+      </c>
+      <c r="W5" s="17">
+        <f>V5*D5</f>
+        <v>0</v>
+      </c>
+      <c r="X5" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="W5" s="1"/>
+      <c r="Y5" s="1"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="14">
+      <c r="B6" s="11"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="13">
         <v>0.375</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="13">
         <v>0.04</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="13">
         <v>0.15</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="13">
         <v>0.1</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6" s="13">
         <v>0.1</v>
       </c>
-      <c r="I6" s="14">
+      <c r="I6" s="13">
         <v>10</v>
       </c>
-      <c r="J6" s="13">
+      <c r="J6" s="12">
         <f>K6*D6*2*PI()/60</f>
-        <v>23.561944901923447</v>
-      </c>
-      <c r="K6" s="40">
-        <v>600</v>
-      </c>
-      <c r="L6" s="20"/>
-      <c r="M6" s="16">
+        <v>15.707963267948966</v>
+      </c>
+      <c r="K6" s="39">
+        <v>400</v>
+      </c>
+      <c r="L6" s="19"/>
+      <c r="M6" s="15">
+        <f>(10*I6)/Q6*D6</f>
+        <v>4.6875</v>
+      </c>
+      <c r="N6" s="44">
+        <v>0.15</v>
+      </c>
+      <c r="O6" s="13">
+        <v>2500</v>
+      </c>
+      <c r="P6" s="13">
         <v>1</v>
       </c>
-      <c r="N6" s="56">
-        <v>1</v>
-      </c>
-      <c r="O6" s="14">
-        <v>2500</v>
-      </c>
-      <c r="P6" s="14">
-        <v>4</v>
-      </c>
-      <c r="Q6" s="17">
+      <c r="Q6" s="13">
+        <v>8</v>
+      </c>
+      <c r="R6" s="16">
+        <f t="shared" si="0"/>
+        <v>12.271846303085129</v>
+      </c>
+      <c r="S6" s="41">
         <f t="shared" si="1"/>
-        <v>24.543692606170257</v>
-      </c>
-      <c r="R6" s="49">
+        <v>100</v>
+      </c>
+      <c r="T6" s="41">
+        <v>6.666666666666667</v>
+      </c>
+      <c r="U6" s="17">
         <f t="shared" si="2"/>
-        <v>10.666666666666666</v>
-      </c>
-      <c r="S6" s="18">
-        <f t="shared" si="3"/>
-        <v>65.453250670241289</v>
-      </c>
-      <c r="T6" s="16">
-        <v>0</v>
-      </c>
-      <c r="U6" s="18">
-        <f>T6*D6</f>
-        <v>0</v>
-      </c>
-      <c r="V6" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="V6" s="15">
+        <v>0</v>
+      </c>
+      <c r="W6" s="17">
+        <f>V6*D6</f>
+        <v>0</v>
+      </c>
+      <c r="X6" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="W6" s="1"/>
+      <c r="Y6" s="1"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="14">
+      <c r="B7" s="11"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="13">
         <v>0.09</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="13">
         <v>0.04</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="13">
         <v>0.15</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G7" s="13">
         <v>0.1</v>
       </c>
-      <c r="H7" s="14">
+      <c r="H7" s="13">
         <v>0.1</v>
       </c>
-      <c r="I7" s="14">
+      <c r="I7" s="13">
         <v>2.5</v>
       </c>
-      <c r="J7" s="13">
-        <f t="shared" ref="J7:J19" si="4">K7*D7*2*PI()/60</f>
-        <v>5.6548667764616276</v>
-      </c>
-      <c r="K7" s="40">
-        <v>600</v>
-      </c>
-      <c r="L7" s="20"/>
-      <c r="M7" s="16">
+      <c r="J7" s="12">
+        <f t="shared" ref="J7:J19" si="3">K7*D7*2*PI()/60</f>
+        <v>3.7699111843077517</v>
+      </c>
+      <c r="K7" s="39">
+        <v>400</v>
+      </c>
+      <c r="L7" s="19"/>
+      <c r="M7" s="11">
+        <v>0</v>
+      </c>
+      <c r="N7" s="12">
+        <v>0.15</v>
+      </c>
+      <c r="O7" s="12">
+        <v>0</v>
+      </c>
+      <c r="P7" s="12">
         <v>1</v>
       </c>
-      <c r="N7" s="56">
-        <v>1</v>
-      </c>
-      <c r="O7" s="14">
-        <v>0</v>
-      </c>
-      <c r="P7" s="14">
-        <v>4</v>
-      </c>
-      <c r="Q7" s="17">
+      <c r="Q7" s="12">
+        <v>0</v>
+      </c>
+      <c r="R7" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S7" s="39">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R7" s="49">
+      <c r="T7" s="39">
+        <v>6.666666666666667</v>
+      </c>
+      <c r="U7" s="19">
         <f t="shared" si="2"/>
-        <v>44.444444444444443</v>
-      </c>
-      <c r="S7" s="18">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="T7" s="16">
-        <v>0</v>
-      </c>
-      <c r="U7" s="18">
-        <f t="shared" ref="U7:U19" si="5">T7*D7</f>
-        <v>0</v>
-      </c>
-      <c r="V7" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="V7" s="15">
+        <v>0</v>
+      </c>
+      <c r="W7" s="17">
+        <f>V7*D7</f>
+        <v>0</v>
+      </c>
+      <c r="X7" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="W7" s="1"/>
+      <c r="Y7" s="1"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="14">
+      <c r="B8" s="11"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="13">
         <v>0.25</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="13">
         <v>0.04</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="13">
         <v>0.05</v>
       </c>
-      <c r="G8" s="14">
+      <c r="G8" s="13">
         <v>0.1</v>
       </c>
-      <c r="H8" s="14">
+      <c r="H8" s="13">
         <v>0.1</v>
       </c>
-      <c r="I8" s="14">
+      <c r="I8" s="13">
         <v>5</v>
       </c>
-      <c r="J8" s="13">
-        <f t="shared" si="4"/>
-        <v>15.707963267948966</v>
-      </c>
-      <c r="K8" s="40">
-        <v>600</v>
-      </c>
-      <c r="L8" s="20"/>
-      <c r="M8" s="16">
+      <c r="J8" s="12">
+        <f t="shared" si="3"/>
+        <v>10.471975511965978</v>
+      </c>
+      <c r="K8" s="39">
+        <v>400</v>
+      </c>
+      <c r="L8" s="19"/>
+      <c r="M8" s="15">
+        <f t="shared" ref="M7:M19" si="4">(10*I8)/Q8*D8</f>
+        <v>1.5625</v>
+      </c>
+      <c r="N8" s="44">
+        <v>0.15</v>
+      </c>
+      <c r="O8" s="13">
+        <v>2500</v>
+      </c>
+      <c r="P8" s="13">
         <v>1</v>
       </c>
-      <c r="N8" s="56">
-        <v>1</v>
-      </c>
-      <c r="O8" s="14">
-        <v>2500</v>
-      </c>
-      <c r="P8" s="14">
-        <v>4</v>
-      </c>
-      <c r="Q8" s="17">
+      <c r="Q8" s="13">
+        <v>8</v>
+      </c>
+      <c r="R8" s="16">
+        <f t="shared" si="0"/>
+        <v>8.1812308687234196</v>
+      </c>
+      <c r="S8" s="41">
         <f t="shared" si="1"/>
-        <v>16.362461737446839</v>
-      </c>
-      <c r="R8" s="49">
+        <v>50</v>
+      </c>
+      <c r="T8" s="41">
+        <v>6.666666666666667</v>
+      </c>
+      <c r="U8" s="17">
         <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
-      <c r="S8" s="18">
-        <f t="shared" si="3"/>
-        <v>65.453250670241289</v>
-      </c>
-      <c r="T8" s="16">
+        <v>10</v>
+      </c>
+      <c r="V8" s="15">
         <v>70</v>
       </c>
-      <c r="U8" s="18">
-        <f t="shared" si="5"/>
+      <c r="W8" s="17">
+        <f>V8*D8</f>
         <v>17.5</v>
       </c>
-      <c r="V8" s="19" t="s">
+      <c r="X8" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="W8" s="1"/>
+      <c r="Y8" s="1"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="14">
+      <c r="B9" s="11"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="13">
         <v>0.25</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="13">
         <v>0.04</v>
       </c>
-      <c r="F9" s="14">
+      <c r="F9" s="13">
         <v>0.17499999999999999</v>
       </c>
-      <c r="G9" s="14">
+      <c r="G9" s="13">
         <v>0.1</v>
       </c>
-      <c r="H9" s="14">
+      <c r="H9" s="13">
         <v>0.1</v>
       </c>
-      <c r="I9" s="14">
+      <c r="I9" s="13">
         <v>2.5</v>
       </c>
-      <c r="J9" s="13">
+      <c r="J9" s="12">
+        <f t="shared" si="3"/>
+        <v>10.471975511965978</v>
+      </c>
+      <c r="K9" s="39">
+        <v>400</v>
+      </c>
+      <c r="L9" s="19"/>
+      <c r="M9" s="15">
         <f t="shared" si="4"/>
-        <v>15.707963267948966</v>
-      </c>
-      <c r="K9" s="40">
-        <v>600</v>
-      </c>
-      <c r="L9" s="20"/>
-      <c r="M9" s="16">
+        <v>0.78125</v>
+      </c>
+      <c r="N9" s="44">
+        <v>0.15</v>
+      </c>
+      <c r="O9" s="13">
+        <v>2500</v>
+      </c>
+      <c r="P9" s="13">
         <v>1</v>
       </c>
-      <c r="N9" s="56">
-        <v>1</v>
-      </c>
-      <c r="O9" s="14">
-        <v>2500</v>
-      </c>
-      <c r="P9" s="14">
-        <v>4</v>
-      </c>
-      <c r="Q9" s="17">
+      <c r="Q9" s="13">
+        <v>8</v>
+      </c>
+      <c r="R9" s="16">
+        <f t="shared" si="0"/>
+        <v>8.1812308687234196</v>
+      </c>
+      <c r="S9" s="41">
         <f t="shared" si="1"/>
-        <v>16.362461737446839</v>
-      </c>
-      <c r="R9" s="49">
+        <v>25</v>
+      </c>
+      <c r="T9" s="41">
+        <v>6.666666666666667</v>
+      </c>
+      <c r="U9" s="17">
         <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
-      <c r="S9" s="18">
-        <f t="shared" si="3"/>
-        <v>65.453250670241289</v>
-      </c>
-      <c r="T9" s="16">
+        <v>10</v>
+      </c>
+      <c r="V9" s="15">
         <v>70</v>
       </c>
-      <c r="U9" s="18">
-        <f t="shared" si="5"/>
+      <c r="W9" s="17">
+        <f>V9*D9</f>
         <v>17.5</v>
       </c>
-      <c r="V9" s="19" t="s">
+      <c r="X9" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="W9" s="1"/>
+      <c r="Y9" s="1"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="14">
+      <c r="B10" s="11"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="13">
         <v>0.3</v>
       </c>
-      <c r="E10" s="14">
+      <c r="E10" s="13">
         <v>0.04</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F10" s="13">
         <v>0.125</v>
       </c>
-      <c r="G10" s="14">
+      <c r="G10" s="13">
         <v>0.1</v>
       </c>
-      <c r="H10" s="14">
+      <c r="H10" s="13">
         <v>1</v>
       </c>
-      <c r="I10" s="14">
+      <c r="I10" s="13">
         <v>5</v>
       </c>
-      <c r="J10" s="13">
+      <c r="J10" s="12">
+        <f t="shared" si="3"/>
+        <v>12.566370614359171</v>
+      </c>
+      <c r="K10" s="39">
+        <v>400</v>
+      </c>
+      <c r="L10" s="19"/>
+      <c r="M10" s="15">
         <f t="shared" si="4"/>
-        <v>18.849555921538759</v>
-      </c>
-      <c r="K10" s="40">
-        <v>600</v>
-      </c>
-      <c r="L10" s="20"/>
-      <c r="M10" s="16">
+        <v>1.875</v>
+      </c>
+      <c r="N10" s="44">
+        <v>0.15</v>
+      </c>
+      <c r="O10" s="13">
+        <v>2500</v>
+      </c>
+      <c r="P10" s="13">
         <v>1</v>
       </c>
-      <c r="N10" s="56">
-        <v>1</v>
-      </c>
-      <c r="O10" s="14">
-        <v>2500</v>
-      </c>
-      <c r="P10" s="14">
-        <v>4</v>
-      </c>
-      <c r="Q10" s="17">
+      <c r="Q10" s="13">
+        <v>8</v>
+      </c>
+      <c r="R10" s="16">
+        <f t="shared" si="0"/>
+        <v>9.8174770424681022</v>
+      </c>
+      <c r="S10" s="41">
         <f t="shared" si="1"/>
-        <v>19.634954084936204</v>
-      </c>
-      <c r="R10" s="49">
+        <v>50</v>
+      </c>
+      <c r="T10" s="41">
+        <v>6.666666666666667</v>
+      </c>
+      <c r="U10" s="17">
         <f t="shared" si="2"/>
-        <v>13.333333333333334</v>
-      </c>
-      <c r="S10" s="18">
-        <f t="shared" si="3"/>
-        <v>65.453250670241289</v>
-      </c>
-      <c r="T10" s="16">
+        <v>10</v>
+      </c>
+      <c r="V10" s="15">
         <v>12</v>
       </c>
-      <c r="U10" s="18">
-        <f t="shared" si="5"/>
+      <c r="W10" s="17">
+        <f>V10*D10</f>
         <v>3.5999999999999996</v>
       </c>
-      <c r="V10" s="19" t="s">
+      <c r="X10" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="W10" s="1"/>
+      <c r="Y10" s="1"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="14">
+      <c r="B11" s="11"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="13">
         <v>1.3</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="13">
         <v>0.2</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="13">
         <v>0.35</v>
       </c>
-      <c r="G11" s="14">
+      <c r="G11" s="13">
         <v>1</v>
       </c>
-      <c r="H11" s="14">
+      <c r="H11" s="13">
         <v>3</v>
       </c>
-      <c r="I11" s="14">
+      <c r="I11" s="13">
         <v>20</v>
       </c>
-      <c r="J11" s="13">
+      <c r="J11" s="12">
+        <f t="shared" si="3"/>
+        <v>54.454272662223076</v>
+      </c>
+      <c r="K11" s="39">
+        <v>400</v>
+      </c>
+      <c r="L11" s="19"/>
+      <c r="M11" s="15">
         <f t="shared" si="4"/>
-        <v>81.681408993334614</v>
-      </c>
-      <c r="K11" s="40">
-        <v>600</v>
-      </c>
-      <c r="L11" s="20"/>
-      <c r="M11" s="16">
-        <v>30</v>
-      </c>
-      <c r="N11" s="56">
+        <v>32.5</v>
+      </c>
+      <c r="N11" s="44">
+        <v>0.15</v>
+      </c>
+      <c r="O11" s="13">
+        <v>2500</v>
+      </c>
+      <c r="P11" s="13">
         <v>1</v>
       </c>
-      <c r="O11" s="14">
+      <c r="Q11" s="13">
+        <v>8</v>
+      </c>
+      <c r="R11" s="16">
+        <f t="shared" si="0"/>
+        <v>42.542400517361777</v>
+      </c>
+      <c r="S11" s="41">
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
-      <c r="P11" s="14">
-        <v>4</v>
-      </c>
-      <c r="Q11" s="17">
-        <f t="shared" si="1"/>
-        <v>6.8067840827778863</v>
-      </c>
-      <c r="R11" s="49">
+      <c r="T11" s="41">
+        <v>6.666666666666667</v>
+      </c>
+      <c r="U11" s="17">
         <f t="shared" si="2"/>
-        <v>92.307692307692307</v>
-      </c>
-      <c r="S11" s="18">
-        <f t="shared" si="3"/>
-        <v>157.0878016085791</v>
-      </c>
-      <c r="T11" s="16">
+        <v>10</v>
+      </c>
+      <c r="V11" s="15">
         <v>100</v>
       </c>
-      <c r="U11" s="18">
-        <f t="shared" si="5"/>
+      <c r="W11" s="17">
+        <f>V11*D11</f>
         <v>130</v>
       </c>
-      <c r="V11" s="19" t="s">
+      <c r="X11" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="W11" s="1"/>
+      <c r="Y11" s="1"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="14">
+      <c r="B12" s="11"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="13">
         <v>0.13</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E12" s="13">
         <v>0.04</v>
       </c>
-      <c r="F12" s="14">
+      <c r="F12" s="13">
         <v>0.05</v>
       </c>
-      <c r="G12" s="14">
+      <c r="G12" s="13">
         <v>0.1</v>
       </c>
-      <c r="H12" s="14">
+      <c r="H12" s="13">
         <v>0.1</v>
       </c>
-      <c r="I12" s="14">
+      <c r="I12" s="13">
         <v>2.5</v>
       </c>
-      <c r="J12" s="13">
+      <c r="J12" s="12">
+        <f t="shared" si="3"/>
+        <v>5.4454272662223087</v>
+      </c>
+      <c r="K12" s="39">
+        <v>400</v>
+      </c>
+      <c r="L12" s="19"/>
+      <c r="M12" s="15">
         <f t="shared" si="4"/>
-        <v>8.1681408993334621</v>
-      </c>
-      <c r="K12" s="40">
-        <v>600</v>
-      </c>
-      <c r="L12" s="20"/>
-      <c r="M12" s="16">
+        <v>0.40625</v>
+      </c>
+      <c r="N12" s="44">
+        <v>0.15</v>
+      </c>
+      <c r="O12" s="13">
+        <v>2500</v>
+      </c>
+      <c r="P12" s="13">
         <v>1</v>
       </c>
-      <c r="N12" s="56">
-        <v>1</v>
-      </c>
-      <c r="O12" s="14">
-        <v>2500</v>
-      </c>
-      <c r="P12" s="14">
-        <v>4</v>
-      </c>
-      <c r="Q12" s="17">
+      <c r="Q12" s="13">
+        <v>8</v>
+      </c>
+      <c r="R12" s="16">
+        <f t="shared" si="0"/>
+        <v>4.2542400517361783</v>
+      </c>
+      <c r="S12" s="41">
         <f t="shared" si="1"/>
-        <v>8.5084801034723565</v>
-      </c>
-      <c r="R12" s="49">
+        <v>25</v>
+      </c>
+      <c r="T12" s="41">
+        <v>6.666666666666667</v>
+      </c>
+      <c r="U12" s="17">
         <f t="shared" si="2"/>
-        <v>30.769230769230766</v>
-      </c>
-      <c r="S12" s="18">
-        <f t="shared" si="3"/>
-        <v>65.453250670241289</v>
-      </c>
-      <c r="T12" s="16">
+        <v>10</v>
+      </c>
+      <c r="V12" s="15">
         <v>50</v>
       </c>
-      <c r="U12" s="18">
-        <f t="shared" si="5"/>
+      <c r="W12" s="17">
+        <f>V12*D12</f>
         <v>6.5</v>
       </c>
-      <c r="V12" s="19" t="s">
+      <c r="X12" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="W12" s="1"/>
+      <c r="Y12" s="1"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="14">
+      <c r="B13" s="11"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="13">
         <v>0.14000000000000001</v>
       </c>
-      <c r="E13" s="14">
+      <c r="E13" s="13">
         <v>0.04</v>
       </c>
-      <c r="F13" s="14">
+      <c r="F13" s="13">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="G13" s="14">
+      <c r="G13" s="13">
         <v>0.1</v>
       </c>
-      <c r="H13" s="14">
+      <c r="H13" s="13">
         <v>0.1</v>
       </c>
-      <c r="I13" s="14">
+      <c r="I13" s="13">
         <v>5</v>
       </c>
-      <c r="J13" s="13">
+      <c r="J13" s="12">
+        <f t="shared" si="3"/>
+        <v>5.8643062867009483</v>
+      </c>
+      <c r="K13" s="39">
+        <v>400</v>
+      </c>
+      <c r="L13" s="19"/>
+      <c r="M13" s="15">
         <f t="shared" si="4"/>
-        <v>8.7964594300514225</v>
-      </c>
-      <c r="K13" s="40">
-        <v>600</v>
-      </c>
-      <c r="L13" s="20"/>
-      <c r="M13" s="16">
+        <v>0.87500000000000011</v>
+      </c>
+      <c r="N13" s="44">
+        <v>0.15</v>
+      </c>
+      <c r="O13" s="13">
+        <v>2500</v>
+      </c>
+      <c r="P13" s="13">
         <v>1</v>
       </c>
-      <c r="N13" s="56">
-        <v>1</v>
-      </c>
-      <c r="O13" s="14">
-        <v>2500</v>
-      </c>
-      <c r="P13" s="14">
-        <v>4</v>
-      </c>
-      <c r="Q13" s="17">
+      <c r="Q13" s="13">
+        <v>8</v>
+      </c>
+      <c r="R13" s="16">
+        <f t="shared" si="0"/>
+        <v>4.5814892864851151</v>
+      </c>
+      <c r="S13" s="41">
         <f t="shared" si="1"/>
-        <v>9.1629785729702302</v>
-      </c>
-      <c r="R13" s="49">
+        <v>50</v>
+      </c>
+      <c r="T13" s="41">
+        <v>6.666666666666667</v>
+      </c>
+      <c r="U13" s="17">
         <f t="shared" si="2"/>
-        <v>28.571428571428569</v>
-      </c>
-      <c r="S13" s="18">
-        <f t="shared" si="3"/>
-        <v>65.453250670241289</v>
-      </c>
-      <c r="T13" s="16">
+        <v>10</v>
+      </c>
+      <c r="V13" s="15">
         <v>50</v>
       </c>
-      <c r="U13" s="18">
-        <f t="shared" si="5"/>
+      <c r="W13" s="17">
+        <f>V13*D13</f>
         <v>7.0000000000000009</v>
       </c>
-      <c r="V13" s="19" t="s">
+      <c r="X13" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="W13" s="1"/>
+      <c r="Y13" s="1"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="14">
+      <c r="B14" s="11"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="13">
         <v>0.16</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14" s="13">
         <v>0.04</v>
       </c>
-      <c r="F14" s="14">
+      <c r="F14" s="13">
         <v>0.1</v>
       </c>
-      <c r="G14" s="14">
+      <c r="G14" s="13">
         <v>0.1</v>
       </c>
-      <c r="H14" s="14">
+      <c r="H14" s="13">
         <v>0.1</v>
       </c>
-      <c r="I14" s="14">
+      <c r="I14" s="13">
         <v>5</v>
       </c>
-      <c r="J14" s="13">
+      <c r="J14" s="12">
+        <f t="shared" si="3"/>
+        <v>6.702064327658225</v>
+      </c>
+      <c r="K14" s="39">
+        <v>400</v>
+      </c>
+      <c r="L14" s="19"/>
+      <c r="M14" s="15">
         <f t="shared" si="4"/>
-        <v>10.053096491487338</v>
-      </c>
-      <c r="K14" s="40">
-        <v>600</v>
-      </c>
-      <c r="L14" s="20"/>
-      <c r="M14" s="16">
         <v>1</v>
       </c>
-      <c r="N14" s="56">
+      <c r="N14" s="44">
+        <v>0.15</v>
+      </c>
+      <c r="O14" s="13">
+        <v>2500</v>
+      </c>
+      <c r="P14" s="13">
         <v>1</v>
       </c>
-      <c r="O14" s="14">
-        <v>2500</v>
-      </c>
-      <c r="P14" s="14">
-        <v>4</v>
-      </c>
-      <c r="Q14" s="17">
+      <c r="Q14" s="13">
+        <v>8</v>
+      </c>
+      <c r="R14" s="16">
+        <f t="shared" si="0"/>
+        <v>5.2359877559829879</v>
+      </c>
+      <c r="S14" s="41">
         <f t="shared" si="1"/>
-        <v>10.471975511965976</v>
-      </c>
-      <c r="R14" s="49">
+        <v>50</v>
+      </c>
+      <c r="T14" s="41">
+        <v>6.666666666666667</v>
+      </c>
+      <c r="U14" s="17">
         <f t="shared" si="2"/>
-        <v>25</v>
-      </c>
-      <c r="S14" s="18">
-        <f t="shared" si="3"/>
-        <v>65.453250670241289</v>
-      </c>
-      <c r="T14" s="16">
+        <v>10</v>
+      </c>
+      <c r="V14" s="15">
         <v>12</v>
       </c>
-      <c r="U14" s="18">
-        <f t="shared" si="5"/>
+      <c r="W14" s="17">
+        <f>V14*D14</f>
         <v>1.92</v>
       </c>
-      <c r="V14" s="19" t="s">
+      <c r="X14" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="W14" s="1"/>
+      <c r="Y14" s="1"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="14">
+      <c r="B15" s="11"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="13">
         <v>0.22</v>
       </c>
-      <c r="E15" s="14">
+      <c r="E15" s="13">
         <v>0.04</v>
       </c>
-      <c r="F15" s="14">
+      <c r="F15" s="13">
         <v>0.14000000000000001</v>
       </c>
-      <c r="G15" s="14">
+      <c r="G15" s="13">
         <v>0.1</v>
       </c>
-      <c r="H15" s="14">
+      <c r="H15" s="13">
         <v>0.1</v>
       </c>
-      <c r="I15" s="14">
+      <c r="I15" s="13">
         <v>2.5</v>
       </c>
-      <c r="J15" s="13">
+      <c r="J15" s="12">
+        <f t="shared" si="3"/>
+        <v>9.2153384505300586</v>
+      </c>
+      <c r="K15" s="39">
+        <v>400</v>
+      </c>
+      <c r="L15" s="19"/>
+      <c r="M15" s="15">
         <f t="shared" si="4"/>
-        <v>13.82300767579509</v>
-      </c>
-      <c r="K15" s="40">
-        <v>600</v>
-      </c>
-      <c r="L15" s="20"/>
-      <c r="M15" s="16">
+        <v>0.6875</v>
+      </c>
+      <c r="N15" s="44">
+        <v>0.15</v>
+      </c>
+      <c r="O15" s="13">
+        <v>2500</v>
+      </c>
+      <c r="P15" s="13">
         <v>1</v>
       </c>
-      <c r="N15" s="56">
-        <v>1</v>
-      </c>
-      <c r="O15" s="14">
-        <v>2500</v>
-      </c>
-      <c r="P15" s="14">
-        <v>4</v>
-      </c>
-      <c r="Q15" s="17">
+      <c r="Q15" s="13">
+        <v>8</v>
+      </c>
+      <c r="R15" s="16">
+        <f t="shared" si="0"/>
+        <v>7.1994831644766091</v>
+      </c>
+      <c r="S15" s="41">
         <f t="shared" si="1"/>
-        <v>14.398966328953218</v>
-      </c>
-      <c r="R15" s="49">
+        <v>25</v>
+      </c>
+      <c r="T15" s="41">
+        <v>6.666666666666667</v>
+      </c>
+      <c r="U15" s="17">
         <f t="shared" si="2"/>
-        <v>18.181818181818183</v>
-      </c>
-      <c r="S15" s="18">
-        <f t="shared" si="3"/>
-        <v>65.453250670241289</v>
-      </c>
-      <c r="T15" s="16">
+        <v>10</v>
+      </c>
+      <c r="V15" s="15">
         <v>12</v>
       </c>
-      <c r="U15" s="18">
-        <f t="shared" si="5"/>
+      <c r="W15" s="17">
+        <f>V15*D15</f>
         <v>2.64</v>
       </c>
-      <c r="V15" s="19" t="s">
+      <c r="X15" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="W15" s="1"/>
+      <c r="Y15" s="1"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="14">
+      <c r="B16" s="11"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="13">
         <v>1.38</v>
       </c>
-      <c r="E16" s="14">
+      <c r="E16" s="13">
         <v>0.25</v>
       </c>
-      <c r="F16" s="14">
+      <c r="F16" s="13">
         <v>0.35</v>
       </c>
-      <c r="G16" s="14">
+      <c r="G16" s="13">
         <v>1</v>
       </c>
-      <c r="H16" s="14">
+      <c r="H16" s="13">
         <v>10</v>
       </c>
-      <c r="I16" s="14">
+      <c r="I16" s="13">
         <v>20</v>
       </c>
-      <c r="J16" s="13">
+      <c r="J16" s="12">
+        <f t="shared" si="3"/>
+        <v>57.805304826052193</v>
+      </c>
+      <c r="K16" s="39">
+        <v>400</v>
+      </c>
+      <c r="L16" s="19"/>
+      <c r="M16" s="15">
         <f t="shared" si="4"/>
-        <v>86.707957239078283</v>
-      </c>
-      <c r="K16" s="40">
-        <v>600</v>
-      </c>
-      <c r="L16" s="20"/>
-      <c r="M16" s="16">
+        <v>34.5</v>
+      </c>
+      <c r="N16" s="44">
+        <v>0.15</v>
+      </c>
+      <c r="O16" s="13">
+        <v>2500</v>
+      </c>
+      <c r="P16" s="13">
         <v>1</v>
       </c>
-      <c r="N16" s="56">
-        <v>1</v>
-      </c>
-      <c r="O16" s="14">
-        <v>2500</v>
-      </c>
-      <c r="P16" s="14">
-        <v>4</v>
-      </c>
-      <c r="Q16" s="17">
+      <c r="Q16" s="13">
+        <v>8</v>
+      </c>
+      <c r="R16" s="16">
+        <f t="shared" si="0"/>
+        <v>45.160394395353272</v>
+      </c>
+      <c r="S16" s="41">
         <f t="shared" si="1"/>
-        <v>90.320788790706544</v>
-      </c>
-      <c r="R16" s="49">
+        <v>200.00000000000003</v>
+      </c>
+      <c r="T16" s="41">
+        <v>6.666666666666667</v>
+      </c>
+      <c r="U16" s="17">
         <f t="shared" si="2"/>
-        <v>2.8985507246376816</v>
-      </c>
-      <c r="S16" s="18">
-        <f t="shared" si="3"/>
-        <v>65.453250670241289</v>
-      </c>
-      <c r="T16" s="16">
+        <v>10.000000000000002</v>
+      </c>
+      <c r="V16" s="15">
         <v>100</v>
       </c>
-      <c r="U16" s="18">
-        <f t="shared" si="5"/>
+      <c r="W16" s="17">
+        <f>V16*D16</f>
         <v>138</v>
       </c>
-      <c r="V16" s="19">
+      <c r="X16" s="18">
         <v>40</v>
       </c>
-      <c r="W16" s="1"/>
+      <c r="Y16" s="1"/>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="14">
+      <c r="B17" s="11"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="13">
         <v>0.52</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E17" s="13">
         <v>0.08</v>
       </c>
-      <c r="F17" s="14">
+      <c r="F17" s="13">
         <v>0.68</v>
       </c>
-      <c r="G17" s="14">
+      <c r="G17" s="13">
         <v>0.5</v>
       </c>
-      <c r="H17" s="14">
+      <c r="H17" s="13">
         <v>2</v>
       </c>
-      <c r="I17" s="14">
+      <c r="I17" s="13">
         <v>10</v>
       </c>
-      <c r="J17" s="13">
+      <c r="J17" s="12">
+        <f t="shared" si="3"/>
+        <v>21.781709064889235</v>
+      </c>
+      <c r="K17" s="39">
+        <v>400</v>
+      </c>
+      <c r="L17" s="19"/>
+      <c r="M17" s="15">
         <f t="shared" si="4"/>
-        <v>32.672563597333848</v>
-      </c>
-      <c r="K17" s="40">
-        <v>600</v>
-      </c>
-      <c r="L17" s="20"/>
-      <c r="M17" s="16">
+        <v>6.5</v>
+      </c>
+      <c r="N17" s="44">
+        <v>0.15</v>
+      </c>
+      <c r="O17" s="13">
+        <v>2500</v>
+      </c>
+      <c r="P17" s="13">
         <v>1</v>
       </c>
-      <c r="N17" s="56">
-        <v>1</v>
-      </c>
-      <c r="O17" s="14">
-        <v>2500</v>
-      </c>
-      <c r="P17" s="14">
-        <v>4</v>
-      </c>
-      <c r="Q17" s="17">
+      <c r="Q17" s="13">
+        <v>8</v>
+      </c>
+      <c r="R17" s="16">
+        <f t="shared" si="0"/>
+        <v>17.016960206944713</v>
+      </c>
+      <c r="S17" s="41">
         <f t="shared" si="1"/>
-        <v>34.033920413889426</v>
-      </c>
-      <c r="R17" s="49">
+        <v>100</v>
+      </c>
+      <c r="T17" s="41">
+        <v>6.666666666666667</v>
+      </c>
+      <c r="U17" s="17">
         <f t="shared" si="2"/>
-        <v>7.6923076923076916</v>
-      </c>
-      <c r="S17" s="18">
-        <f t="shared" si="3"/>
-        <v>65.453250670241289</v>
-      </c>
-      <c r="T17" s="16">
+        <v>10</v>
+      </c>
+      <c r="V17" s="15">
         <v>80</v>
       </c>
-      <c r="U17" s="18">
-        <f t="shared" si="5"/>
+      <c r="W17" s="17">
+        <f>V17*D17</f>
         <v>41.6</v>
       </c>
-      <c r="V17" s="19">
+      <c r="X17" s="18">
         <v>20</v>
       </c>
-      <c r="W17" s="1"/>
+      <c r="Y17" s="1"/>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="14">
+      <c r="B18" s="11"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="13">
         <v>0.34399999999999997</v>
       </c>
-      <c r="E18" s="14">
+      <c r="E18" s="13">
         <v>0.04</v>
       </c>
-      <c r="F18" s="14">
+      <c r="F18" s="13">
         <v>0.21</v>
       </c>
-      <c r="G18" s="14">
+      <c r="G18" s="13">
         <v>0.1</v>
       </c>
-      <c r="H18" s="14">
+      <c r="H18" s="13">
         <v>1</v>
       </c>
-      <c r="I18" s="14">
+      <c r="I18" s="13">
         <v>5</v>
       </c>
-      <c r="J18" s="13">
+      <c r="J18" s="12">
+        <f t="shared" si="3"/>
+        <v>14.409438304465185</v>
+      </c>
+      <c r="K18" s="39">
+        <v>400</v>
+      </c>
+      <c r="L18" s="19"/>
+      <c r="M18" s="15">
         <f t="shared" si="4"/>
-        <v>21.614157456697775</v>
-      </c>
-      <c r="K18" s="40">
-        <v>600</v>
-      </c>
-      <c r="L18" s="20"/>
-      <c r="M18" s="16">
+        <v>2.15</v>
+      </c>
+      <c r="N18" s="44">
+        <v>0.15</v>
+      </c>
+      <c r="O18" s="13">
+        <v>2500</v>
+      </c>
+      <c r="P18" s="13">
         <v>1</v>
       </c>
-      <c r="N18" s="56">
-        <v>1</v>
-      </c>
-      <c r="O18" s="14">
-        <v>2500</v>
-      </c>
-      <c r="P18" s="14">
-        <v>4</v>
-      </c>
-      <c r="Q18" s="17">
+      <c r="Q18" s="13">
+        <v>8</v>
+      </c>
+      <c r="R18" s="16">
+        <f t="shared" si="0"/>
+        <v>11.257373675363425</v>
+      </c>
+      <c r="S18" s="41">
         <f t="shared" si="1"/>
-        <v>22.51474735072685</v>
-      </c>
-      <c r="R18" s="49">
+        <v>50</v>
+      </c>
+      <c r="T18" s="41">
+        <v>6.666666666666667</v>
+      </c>
+      <c r="U18" s="17">
         <f t="shared" si="2"/>
-        <v>11.627906976744187</v>
-      </c>
-      <c r="S18" s="18">
-        <f t="shared" si="3"/>
-        <v>65.453250670241289</v>
-      </c>
-      <c r="T18" s="16">
+        <v>10</v>
+      </c>
+      <c r="V18" s="15">
         <v>12</v>
       </c>
-      <c r="U18" s="18">
-        <f t="shared" si="5"/>
+      <c r="W18" s="17">
+        <f>V18*D18</f>
         <v>4.1280000000000001</v>
       </c>
-      <c r="V18" s="19">
+      <c r="X18" s="18">
         <v>40</v>
       </c>
-      <c r="W18" s="1"/>
+      <c r="Y18" s="1"/>
     </row>
-    <row r="19" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="23">
+      <c r="B19" s="20"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="22">
         <v>0.21</v>
       </c>
-      <c r="E19" s="23">
+      <c r="E19" s="22">
         <v>0.04</v>
       </c>
-      <c r="F19" s="23">
+      <c r="F19" s="22">
         <v>0.1</v>
       </c>
-      <c r="G19" s="23">
+      <c r="G19" s="22">
         <v>0.1</v>
       </c>
-      <c r="H19" s="23">
+      <c r="H19" s="22">
         <v>0.5</v>
       </c>
-      <c r="I19" s="23">
+      <c r="I19" s="22">
         <v>2</v>
       </c>
-      <c r="J19" s="22">
+      <c r="J19" s="21">
+        <f t="shared" si="3"/>
+        <v>8.7964594300514207</v>
+      </c>
+      <c r="K19" s="21">
+        <v>400</v>
+      </c>
+      <c r="L19" s="23"/>
+      <c r="M19" s="24">
         <f t="shared" si="4"/>
-        <v>13.194689145077131</v>
-      </c>
-      <c r="K19" s="41">
-        <v>600</v>
-      </c>
-      <c r="L19" s="24"/>
-      <c r="M19" s="25">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="N19" s="45">
+        <v>0.15</v>
+      </c>
+      <c r="O19" s="22">
+        <v>2500</v>
+      </c>
+      <c r="P19" s="22">
         <v>1</v>
       </c>
-      <c r="N19" s="57">
-        <v>1</v>
-      </c>
-      <c r="O19" s="23">
-        <v>2500</v>
-      </c>
-      <c r="P19" s="23">
-        <v>4</v>
-      </c>
-      <c r="Q19" s="26">
+      <c r="Q19" s="22">
+        <v>8</v>
+      </c>
+      <c r="R19" s="25">
+        <f t="shared" si="0"/>
+        <v>6.8722339297276722</v>
+      </c>
+      <c r="S19" s="42">
         <f t="shared" si="1"/>
-        <v>13.744467859455344</v>
-      </c>
-      <c r="R19" s="50">
+        <v>20</v>
+      </c>
+      <c r="T19" s="42">
+        <v>6.666666666666667</v>
+      </c>
+      <c r="U19" s="26">
         <f t="shared" si="2"/>
-        <v>19.047619047619047</v>
-      </c>
-      <c r="S19" s="27">
-        <f t="shared" si="3"/>
-        <v>65.453250670241289</v>
-      </c>
-      <c r="T19" s="25">
+        <v>10</v>
+      </c>
+      <c r="V19" s="24">
         <v>80</v>
       </c>
-      <c r="U19" s="27">
-        <f t="shared" si="5"/>
+      <c r="W19" s="26">
+        <f>V19*D19</f>
         <v>16.8</v>
       </c>
-      <c r="V19" s="28" t="s">
+      <c r="X19" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="W19" s="2"/>
+      <c r="Y19" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B1:L1"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="W1:W2"/>
-    <mergeCell ref="M1:S1"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="Y1:Y2"/>
+    <mergeCell ref="M1:U1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>